<commit_message>
Pass rng to background and add test
</commit_message>
<xml_diff>
--- a/tests/data/config/design_input_background.xlsx
+++ b/tests/data/config/design_input_background.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\fmu\users\tral\fmu-utils\github\fmu-tools\tests\data\sensitivities\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FCUR/git/fmu-tools/tests/sensitivities/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76DC316-38E3-4369-BD57-DD8BC15A4DC9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F818A72B-633D-8F4D-A600-F8B4ADA22047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="2055" windowWidth="27240" windowHeight="6570" tabRatio="992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16340" yWindow="5100" windowWidth="37220" windowHeight="24200" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -464,9 +464,6 @@
     <t>PARAM13</t>
   </si>
   <si>
-    <t>tests/data/sensitivities/config/doe1.xlsx</t>
-  </si>
-  <si>
     <t>PARAM14</t>
   </si>
   <si>
@@ -519,6 +516,9 @@
   </si>
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>doe1.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1364,10 +1364,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="193">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1402,13 +1402,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1429,13 +1429,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1456,14 +1456,14 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1486,13 +1486,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1517,9 +1517,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1532,7 +1532,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1545,8 +1545,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1567,20 +1567,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1593,17 +1593,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1621,20 +1621,20 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1646,16 +1646,16 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="53" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1665,43 +1665,42 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="55" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="40" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="56" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="44" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="45" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="46" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="47" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="48" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="50" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="51" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="52" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1732,9 +1731,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="46" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="50" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="58" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1748,16 +1744,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2403,9 +2396,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2443,7 +2436,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2549,7 +2542,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2691,7 +2684,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2701,19 +2694,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="77.85546875"/>
-    <col min="4" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="10.83203125"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77.83203125"/>
+    <col min="4" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2721,7 +2714,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2729,15 +2722,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -2757,30 +2750,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.85546875"/>
+    <col min="1" max="1" width="10.83203125"/>
     <col min="2" max="2" width="10"/>
-    <col min="3" max="3" width="12.5703125"/>
-    <col min="4" max="4" width="11.85546875"/>
+    <col min="3" max="3" width="12.5"/>
+    <col min="4" max="4" width="11.83203125"/>
     <col min="5" max="5" width="10" style="2"/>
-    <col min="6" max="8" width="11.85546875" style="2"/>
-    <col min="9" max="9" width="11.85546875"/>
-    <col min="10" max="10" width="33.140625" style="2"/>
-    <col min="11" max="14" width="11.85546875" style="2"/>
-    <col min="15" max="17" width="11.85546875"/>
-    <col min="18" max="19" width="8.7109375"/>
-    <col min="20" max="20" width="9.85546875"/>
-    <col min="21" max="21" width="8.7109375"/>
-    <col min="22" max="22" width="9.85546875"/>
-    <col min="23" max="1025" width="8.7109375"/>
+    <col min="6" max="8" width="11.83203125" style="2"/>
+    <col min="9" max="9" width="11.83203125"/>
+    <col min="10" max="10" width="33.1640625" style="2"/>
+    <col min="11" max="14" width="11.83203125" style="2"/>
+    <col min="15" max="17" width="11.83203125"/>
+    <col min="18" max="19" width="8.6640625"/>
+    <col min="20" max="20" width="9.83203125"/>
+    <col min="21" max="21" width="8.6640625"/>
+    <col min="22" max="22" width="9.83203125"/>
+    <col min="23" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
@@ -2831,7 +2824,7 @@
       </c>
       <c r="V1" s="1"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>3</v>
       </c>
@@ -2853,7 +2846,7 @@
       <c r="O2" s="28"/>
       <c r="P2" s="29"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="30" t="s">
         <v>20</v>
       </c>
@@ -2885,7 +2878,7 @@
       <c r="O3" s="41"/>
       <c r="P3" s="42"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="43" t="s">
         <v>25</v>
       </c>
@@ -2913,7 +2906,7 @@
       <c r="O4" s="55"/>
       <c r="P4" s="56"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
         <v>28</v>
       </c>
@@ -2945,7 +2938,7 @@
       <c r="O5" s="68"/>
       <c r="P5" s="69"/>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" s="70"/>
       <c r="B6" s="71"/>
       <c r="C6" s="72"/>
@@ -2969,7 +2962,7 @@
       <c r="O6" s="81"/>
       <c r="P6" s="82"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" s="83"/>
       <c r="B7" s="84"/>
       <c r="C7" s="85"/>
@@ -2993,7 +2986,7 @@
       <c r="O7" s="94"/>
       <c r="P7" s="95"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" s="96" t="s">
         <v>34</v>
       </c>
@@ -3025,7 +3018,7 @@
       <c r="O8" s="102"/>
       <c r="P8" s="107"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" s="108" t="s">
         <v>39</v>
       </c>
@@ -3061,7 +3054,7 @@
       <c r="O9" s="114"/>
       <c r="P9" s="119"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="120"/>
       <c r="B10" s="121"/>
       <c r="C10" s="122"/>
@@ -3087,7 +3080,7 @@
       <c r="O10" s="126"/>
       <c r="P10" s="131"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A11" s="120"/>
       <c r="B11" s="121"/>
       <c r="C11" s="122"/>
@@ -3115,7 +3108,7 @@
       <c r="O11" s="126"/>
       <c r="P11" s="131"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A12" s="132"/>
       <c r="B12" s="133"/>
       <c r="C12" s="134"/>
@@ -3141,7 +3134,7 @@
       <c r="O12" s="138"/>
       <c r="P12" s="143"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A13" s="144" t="s">
         <v>50</v>
       </c>
@@ -3177,14 +3170,14 @@
       </c>
       <c r="P13" s="156"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A14" s="144"/>
       <c r="B14" s="145"/>
       <c r="C14" s="146"/>
       <c r="D14" s="147" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="157"/>
+      <c r="E14" s="148"/>
       <c r="F14" s="145"/>
       <c r="G14" s="145"/>
       <c r="H14" s="149"/>
@@ -3207,14 +3200,14 @@
       </c>
       <c r="P14" s="156"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A15" s="144"/>
       <c r="B15" s="145"/>
       <c r="C15" s="146"/>
       <c r="D15" s="147" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="157"/>
+      <c r="E15" s="148"/>
       <c r="F15" s="145"/>
       <c r="G15" s="145"/>
       <c r="H15" s="149"/>
@@ -3237,35 +3230,35 @@
       </c>
       <c r="P15" s="156"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A16" s="158"/>
-      <c r="B16" s="159"/>
-      <c r="C16" s="160"/>
-      <c r="D16" s="161" t="s">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A16" s="157"/>
+      <c r="B16" s="158"/>
+      <c r="C16" s="159"/>
+      <c r="D16" s="160" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="162"/>
-      <c r="F16" s="159"/>
-      <c r="G16" s="159"/>
-      <c r="H16" s="163"/>
-      <c r="I16" s="164" t="s">
+      <c r="E16" s="161"/>
+      <c r="F16" s="158"/>
+      <c r="G16" s="158"/>
+      <c r="H16" s="162"/>
+      <c r="I16" s="163" t="s">
         <v>37</v>
       </c>
-      <c r="J16" s="165">
+      <c r="J16" s="164">
         <v>1</v>
       </c>
-      <c r="K16" s="166">
+      <c r="K16" s="165">
         <v>10</v>
       </c>
-      <c r="L16" s="167"/>
-      <c r="M16" s="168"/>
-      <c r="N16" s="168"/>
+      <c r="L16" s="166"/>
+      <c r="M16" s="167"/>
+      <c r="N16" s="167"/>
       <c r="O16" s="155" t="s">
         <v>53</v>
       </c>
       <c r="P16" s="156"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A17" s="108" t="s">
         <v>57</v>
       </c>
@@ -3278,79 +3271,79 @@
       <c r="D17" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="169"/>
-      <c r="F17" s="170"/>
-      <c r="G17" s="170"/>
-      <c r="H17" s="171"/>
+      <c r="E17" s="168"/>
+      <c r="F17" s="169"/>
+      <c r="G17" s="169"/>
+      <c r="H17" s="170"/>
       <c r="I17" s="114"/>
       <c r="J17" s="115"/>
       <c r="K17" s="116"/>
       <c r="L17" s="117"/>
       <c r="M17" s="118"/>
       <c r="N17" s="118"/>
-      <c r="O17" s="172"/>
+      <c r="O17" s="171"/>
       <c r="P17" s="119" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="120"/>
       <c r="B18" s="121"/>
       <c r="C18" s="122"/>
       <c r="D18" s="123" t="s">
-        <v>61</v>
-      </c>
-      <c r="E18" s="173"/>
-      <c r="F18" s="174"/>
-      <c r="G18" s="174"/>
-      <c r="H18" s="175"/>
+        <v>60</v>
+      </c>
+      <c r="E18" s="172"/>
+      <c r="F18" s="173"/>
+      <c r="G18" s="173"/>
+      <c r="H18" s="174"/>
       <c r="I18" s="126"/>
       <c r="J18" s="127"/>
       <c r="K18" s="128"/>
       <c r="L18" s="129"/>
       <c r="M18" s="130"/>
       <c r="N18" s="130"/>
-      <c r="O18" s="176"/>
+      <c r="O18" s="175"/>
       <c r="P18" s="131"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="120"/>
       <c r="B19" s="121"/>
       <c r="C19" s="122"/>
       <c r="D19" s="123" t="s">
-        <v>62</v>
-      </c>
-      <c r="E19" s="173"/>
-      <c r="F19" s="174"/>
-      <c r="G19" s="174"/>
-      <c r="H19" s="175"/>
+        <v>61</v>
+      </c>
+      <c r="E19" s="172"/>
+      <c r="F19" s="173"/>
+      <c r="G19" s="173"/>
+      <c r="H19" s="174"/>
       <c r="I19" s="126"/>
       <c r="J19" s="127"/>
       <c r="K19" s="128"/>
       <c r="L19" s="129"/>
       <c r="M19" s="130"/>
       <c r="N19" s="130"/>
-      <c r="O19" s="176"/>
+      <c r="O19" s="175"/>
       <c r="P19" s="131"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A20" s="132"/>
       <c r="B20" s="133"/>
       <c r="C20" s="134"/>
       <c r="D20" s="135" t="s">
-        <v>63</v>
-      </c>
-      <c r="E20" s="177"/>
-      <c r="F20" s="178"/>
-      <c r="G20" s="178"/>
-      <c r="H20" s="179"/>
+        <v>62</v>
+      </c>
+      <c r="E20" s="176"/>
+      <c r="F20" s="177"/>
+      <c r="G20" s="177"/>
+      <c r="H20" s="178"/>
       <c r="I20" s="138"/>
       <c r="J20" s="139"/>
       <c r="K20" s="140"/>
       <c r="L20" s="141"/>
       <c r="M20" s="142"/>
       <c r="N20" s="142"/>
-      <c r="O20" s="180"/>
+      <c r="O20" s="179"/>
       <c r="P20" s="143"/>
     </row>
   </sheetData>
@@ -3369,46 +3362,46 @@
       <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5703125"/>
-    <col min="2" max="2" width="13.42578125" style="2"/>
-    <col min="3" max="1025" width="8.7109375"/>
+    <col min="1" max="1" width="12.5"/>
+    <col min="2" max="2" width="13.5" style="2"/>
+    <col min="3" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>65</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>68</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -3416,15 +3409,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>26</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -3432,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3440,7 +3433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3448,15 +3441,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -3464,7 +3457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>42</v>
       </c>
@@ -3472,7 +3465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -3480,15 +3473,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -3496,7 +3489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>54</v>
       </c>
@@ -3504,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>55</v>
       </c>
@@ -3512,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>56</v>
       </c>
@@ -3520,7 +3513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -3528,60 +3521,60 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B22" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>46</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3600,12 +3593,12 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375"/>
+    <col min="1" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>51</v>
       </c>
@@ -3619,59 +3612,59 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="181">
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
-      <c r="E2" s="181"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="181" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="181">
+      <c r="B3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="181">
+      <c r="B4" s="2">
         <v>0</v>
       </c>
-      <c r="C4" s="181" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="181">
+      <c r="C4" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="2">
         <v>1</v>
       </c>
-      <c r="E4" s="181"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="181">
+      <c r="B5" s="2">
         <v>0</v>
       </c>
-      <c r="C5" s="181">
+      <c r="C5" s="2">
         <v>0</v>
       </c>
-      <c r="D5" s="181">
+      <c r="D5" s="2">
         <v>0</v>
       </c>
-      <c r="E5" s="181">
+      <c r="E5" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3689,106 +3682,105 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="11.5703125"/>
-    <col min="7" max="7" width="8.85546875"/>
-    <col min="8" max="8" width="15.28515625"/>
-    <col min="9" max="1025" width="11.5703125"/>
+    <col min="1" max="6" width="11.5"/>
+    <col min="8" max="8" width="15.33203125"/>
+    <col min="9" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="182" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="180" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="183" t="s">
+      <c r="B1" s="181" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="184" t="s">
+      <c r="C1" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="185" t="s">
+      <c r="D1" s="183" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="185" t="s">
+      <c r="E1" s="183" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="185" t="s">
+      <c r="F1" s="183" t="s">
         <v>16</v>
       </c>
-      <c r="G1" s="185" t="s">
+      <c r="G1" s="183" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="186" t="s">
+      <c r="H1" s="184" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="187" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="185" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="186" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="187">
+        <v>0</v>
+      </c>
+      <c r="D2" s="187">
+        <v>1</v>
+      </c>
+      <c r="E2" s="187"/>
+      <c r="F2" s="187"/>
+      <c r="G2" s="187">
+        <v>2</v>
+      </c>
+      <c r="H2" s="155" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="188" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="188" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="189">
+      <c r="B3" s="189" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="189">
+      <c r="D3" s="2">
         <v>1</v>
       </c>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189">
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
         <v>2</v>
       </c>
-      <c r="H2" s="155" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="190" t="s">
+      <c r="H3" s="155" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="188" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="191" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="192">
-        <v>0</v>
-      </c>
-      <c r="D3" s="192">
+      <c r="B4" s="189" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192">
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
         <v>2</v>
       </c>
-      <c r="H3" s="155" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="190" t="s">
-        <v>74</v>
-      </c>
-      <c r="B4" s="191" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="192">
-        <v>1</v>
-      </c>
-      <c r="D4" s="192">
-        <v>3</v>
-      </c>
-      <c r="E4" s="192">
-        <v>5</v>
-      </c>
-      <c r="F4" s="192"/>
-      <c r="G4" s="192">
-        <v>2</v>
-      </c>
       <c r="H4" s="155" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -3811,55 +3803,55 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1025" width="8.7109375"/>
+    <col min="1" max="1025" width="8.6640625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" t="s">
         <v>72</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>73</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B2" s="181">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="C2" s="181"/>
-      <c r="D2" s="181"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="D3" s="2"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>73</v>
       </c>
-      <c r="B3" s="181" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="181">
-        <v>1</v>
-      </c>
-      <c r="D3" s="181"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="181">
-        <v>0</v>
-      </c>
-      <c r="C4" s="181" t="s">
-        <v>75</v>
-      </c>
-      <c r="D4" s="181">
+      <c r="D4" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Test that vars are correlated (#245)
Increased numreal to 500 for correlated samples in
design_input_background.xlsx

Change PARAM11 from Triangle(1, 1, 1) to Triangle(0, 0.5, 1).

---------

Co-authored-by: Sondre Sortland <sondreso@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/tests/data/config/design_input_background.xlsx
+++ b/tests/data/config/design_input_background.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FCUR/git/fmu-tools/tests/sensitivities/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F818A72B-633D-8F4D-A600-F8B4ADA22047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFA1221-5FDB-3C4B-BC4E-DD36F86EA8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16340" yWindow="5100" windowWidth="37220" windowHeight="24200" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15380" yWindow="32760" windowWidth="30240" windowHeight="18880" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="background" sheetId="5" r:id="rId5"/>
     <sheet name="background_corr" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -2751,7 +2751,7 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3139,7 +3139,7 @@
         <v>50</v>
       </c>
       <c r="B13" s="145">
-        <v>30</v>
+        <v>500</v>
       </c>
       <c r="C13" s="146" t="s">
         <v>35</v>
@@ -3215,10 +3215,10 @@
         <v>45</v>
       </c>
       <c r="J15" s="151">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K15" s="152">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="L15" s="153">
         <v>1</v>
@@ -3590,7 +3590,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C4" activeCellId="1" sqref="C1 C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Do not sample from multivariate_normal in test
Instead, add correlated PARAM5 ~ TruncatedNormal(3, 1, 1, 5) and PARAM6 ~ Uniform(0, 1) to design_input_background.xlsx.
We don't want tests that call rng.multivariate_normal directly as that will change when we do latin hypercube sampling instead.
Add check that lower bound must be less than upper bound in truncated normal
</commit_message>
<xml_diff>
--- a/tests/data/config/design_input_background.xlsx
+++ b/tests/data/config/design_input_background.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/FCUR/git/fmu-tools/tests/sensitivities/data/config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFA1221-5FDB-3C4B-BC4E-DD36F86EA8BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656DA750-A316-754B-9249-B3C71ED12A51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15380" yWindow="32760" windowWidth="30240" windowHeight="18880" tabRatio="992" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15380" yWindow="34600" windowWidth="30240" windowHeight="18880" tabRatio="992" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" r:id="rId1"/>
     <sheet name="designinput" sheetId="2" r:id="rId2"/>
     <sheet name="defaultvalues" sheetId="3" r:id="rId3"/>
-    <sheet name="corr1" sheetId="4" r:id="rId4"/>
-    <sheet name="background" sheetId="5" r:id="rId5"/>
-    <sheet name="background_corr" sheetId="6" r:id="rId6"/>
+    <sheet name="corr0" sheetId="7" r:id="rId4"/>
+    <sheet name="corr1" sheetId="4" r:id="rId5"/>
+    <sheet name="background" sheetId="5" r:id="rId6"/>
+    <sheet name="background_corr" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -282,7 +283,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="80">
   <si>
     <t>designtype</t>
   </si>
@@ -519,6 +520,9 @@
   </si>
   <si>
     <t>doe1.xlsx</t>
+  </si>
+  <si>
+    <t>corr0</t>
   </si>
 </sst>
 </file>
@@ -2750,8 +2754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3023,7 +3027,7 @@
         <v>39</v>
       </c>
       <c r="B9" s="109">
-        <v>10</v>
+        <v>500</v>
       </c>
       <c r="C9" s="110" t="s">
         <v>35</v>
@@ -3051,7 +3055,9 @@
         <v>5</v>
       </c>
       <c r="N9" s="118"/>
-      <c r="O9" s="114"/>
+      <c r="O9" s="114" t="s">
+        <v>79</v>
+      </c>
       <c r="P9" s="119"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.2">
@@ -3077,7 +3083,9 @@
       <c r="L10" s="129"/>
       <c r="M10" s="130"/>
       <c r="N10" s="130"/>
-      <c r="O10" s="126"/>
+      <c r="O10" s="126" t="s">
+        <v>79</v>
+      </c>
       <c r="P10" s="131"/>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -3586,6 +3594,48 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F3D6AD-89C3-1641-9CBF-9EF76F0F510F}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3">
+        <v>0.8</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
@@ -3674,7 +3724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
@@ -3795,7 +3845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>

</xml_diff>